<commit_message>
final changes to the paper
</commit_message>
<xml_diff>
--- a/Studie/Logfiles-Auswertung.xlsx
+++ b/Studie/Logfiles-Auswertung.xlsx
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="167">
-  <si>
-    <t>Errorrate</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="175">
   <si>
     <t>Angle at Element 1</t>
   </si>
@@ -516,6 +513,33 @@
   </si>
   <si>
     <t>2min 13sek</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>Avg. Hitpoint</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>180 - 100</t>
+  </si>
+  <si>
+    <t>100 - 80</t>
+  </si>
+  <si>
+    <t>80 - 0</t>
+  </si>
+  <si>
+    <t>0 - 85</t>
+  </si>
+  <si>
+    <t>95 - 85</t>
+  </si>
+  <si>
+    <t>100 - 95</t>
   </si>
 </sst>
 </file>
@@ -872,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="M4" sqref="J2:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,286 +908,297 @@
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>33.33</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="J3" t="s">
+        <v>166</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>33.33</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="J4" t="s">
+        <v>167</v>
+      </c>
+      <c r="K4" s="2">
+        <v>110.43</v>
+      </c>
+      <c r="L4" s="2">
+        <v>92.54</v>
+      </c>
+      <c r="M4" s="2">
+        <v>75.63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>13.33</v>
-      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>6.67</v>
-      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>6.67</v>
-      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>13.33</v>
-      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="1">
-        <v>18.100000000000001</v>
-      </c>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -1172,108 +1207,108 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E23" s="2">
         <v>6</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="3">
@@ -1281,7 +1316,7 @@
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -1289,7 +1324,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -1303,7 +1338,7 @@
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -1317,7 +1352,7 @@
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1329,7 +1364,7 @@
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1341,7 +1376,7 @@
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1353,7 +1388,7 @@
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1365,7 +1400,7 @@
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1377,7 +1412,7 @@
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1389,7 +1424,7 @@
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -1401,7 +1436,7 @@
     <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -1413,7 +1448,7 @@
     <row r="36" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1425,7 +1460,7 @@
     <row r="37" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -1437,7 +1472,7 @@
     <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -1449,7 +1484,7 @@
     <row r="39" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -1461,7 +1496,7 @@
     <row r="40" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -1473,7 +1508,7 @@
     <row r="41" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -1485,7 +1520,7 @@
     <row r="42" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -1499,7 +1534,7 @@
         <v>110.43</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -1526,516 +1561,503 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L3" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="M3" s="2">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
+        <v>166</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
+        <v>167</v>
+      </c>
+      <c r="L5" s="2">
+        <v>108.97</v>
+      </c>
+      <c r="M5" s="2">
+        <v>97.29</v>
+      </c>
+      <c r="N5">
+        <v>88.91</v>
+      </c>
+      <c r="O5" s="2">
+        <v>78.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>13.33</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>33.33</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>40</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>26.67</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3">
-        <v>24.8</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2">
+      <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>133</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3">
+      <c r="G20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C21" s="3">
         <v>108.97</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3">
+      <c r="D21" s="2"/>
+      <c r="E21" s="3">
         <v>97.29</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="G22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2">
+      <c r="C23" s="2">
         <v>3</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2">
         <v>17</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="3">
         <v>78.67</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="G24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2044,27 +2066,25 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2">
+      <c r="I25" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="3">
+      <c r="G26" s="3">
         <v>88.91</v>
       </c>
+      <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H28" s="2">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="2">
         <v>5</v>
       </c>
     </row>

</xml_diff>